<commit_message>
fixed error in test - HOWAREYOU - two HOWAREYOU intents
</commit_message>
<xml_diff>
--- a/tests/data/xls/E_EN_master.xlsx
+++ b/tests/data/xls/E_EN_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tom\Watson\workspaces\watson-assistant-workbench\app_example\en_app\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tom\Watson\public_workspaces\watson-assistant-workbench\tests\data\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7020F171-A8CE-442C-8D51-CE6C2AEA8C8F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E175DE2-5B8C-4444-A04F-4BAB843422F5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13812" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13812" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PERSONA-EN" sheetId="14" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>Are you old?</t>
   </si>
   <si>
-    <t>How are you?</t>
-  </si>
-  <si>
     <t>How is it going?</t>
   </si>
   <si>
@@ -1130,6 +1127,9 @@
   </si>
   <si>
     <t>Please ask me questions about ....</t>
+  </si>
+  <si>
+    <t>How are you mate?</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1508,139 +1508,139 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" t="s">
         <v>309</v>
-      </c>
-      <c r="B3" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>322</v>
+      </c>
+      <c r="B11" t="s">
         <v>323</v>
-      </c>
-      <c r="B11" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B12" t="s">
         <v>324</v>
-      </c>
-      <c r="B12" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>324</v>
+      </c>
+      <c r="B13" t="s">
         <v>325</v>
-      </c>
-      <c r="B13" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>333</v>
+      </c>
+      <c r="B23" t="s">
         <v>334</v>
-      </c>
-      <c r="B23" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>316</v>
+      </c>
+      <c r="B25" t="s">
         <v>317</v>
-      </c>
-      <c r="B25" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1731,55 +1731,55 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>23</v>
+        <v>366</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B47" s="1"/>
     </row>
@@ -1789,45 +1789,45 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53" s="1"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B54" s="1"/>
     </row>
@@ -1837,15 +1837,15 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" s="1"/>
     </row>
@@ -1858,20 +1858,20 @@
         <v>16</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B61" s="1"/>
     </row>
@@ -1881,31 +1881,31 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B66" s="1"/>
     </row>
@@ -1915,37 +1915,37 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B71" s="1"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B72" s="1"/>
     </row>
@@ -1955,24 +1955,24 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1981,31 +1981,31 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B81" s="1"/>
     </row>
@@ -2015,15 +2015,15 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B84" s="1"/>
     </row>
@@ -2033,51 +2033,51 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B90" s="1"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B91" s="1"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B92" s="1"/>
     </row>
@@ -2087,33 +2087,33 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B95" s="1"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B96" s="1"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B97" s="1"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B98" s="1"/>
     </row>
@@ -2123,27 +2123,27 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B101" s="2"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B102" s="1"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B103" s="1"/>
     </row>
@@ -2153,43 +2153,43 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B107" s="1"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B110" s="1"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B111" s="1"/>
     </row>
@@ -2199,10 +2199,10 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2211,27 +2211,27 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B116" s="1"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B117" s="1"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B118" s="1"/>
     </row>
@@ -2241,46 +2241,46 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B121" s="2"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B122" s="1"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B123" s="1"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B125" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0"/>
+    <sheetView topLeftCell="A199" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2302,231 +2302,231 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2536,292 +2536,292 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>5</v>
@@ -2829,274 +2829,274 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>1</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>2</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>3</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>4</v>
@@ -3128,206 +3128,206 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B186" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B187" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>